<commit_message>
Working on writeup, experimenting with C
</commit_message>
<xml_diff>
--- a/Desktop Data Arithmetic.xlsx
+++ b/Desktop Data Arithmetic.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="CT-Log 2016-11-21 20-31-16" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -123,13 +123,13 @@
     <t>FLOPS</t>
   </si>
   <si>
-    <t xml:space="preserve">Megaflops = </t>
-  </si>
-  <si>
     <t xml:space="preserve">Average power = </t>
   </si>
   <si>
     <t>FLOPS per Watt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MegaFLOPS = </t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -619,7 +619,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -693,6 +693,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Desktop,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> High Arithmetic Intensity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -756,10 +786,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$110</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>42695.855162037034</c:v>
                 </c:pt>
@@ -1062,136 +1092,16 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>42695.866736111115</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>42695.866851851853</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>42695.866967592592</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>42695.867083333331</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>42695.867199074077</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>42695.867314814815</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>42695.867430555554</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>42695.867546296293</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>42695.867662037039</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>42695.867777777778</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>42695.867893518516</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>42695.868009259262</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>42695.868125000001</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>42695.86824074074</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>42695.868356481478</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>42695.868472222224</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>42695.868587962963</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>42695.868703703702</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>42695.868819444448</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>42695.868935185186</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>42695.869050925925</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>42695.869166666664</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>42695.86928240741</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>42695.869398148148</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>42695.869513888887</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>42695.869629629633</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>42695.869745370372</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>42695.86986111111</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>42695.869976851849</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>42695.870092592595</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>42695.870208333334</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>42695.870324074072</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>42695.870439814818</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>42695.870555555557</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>42695.870671296296</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>42695.870787037034</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>42695.87090277778</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>42695.871018518519</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>42695.871134259258</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>42695.871249999997</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>42695.871365740742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$Q$10:$Q$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$Q$10:$Q$110</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>66</c:v>
                 </c:pt>
@@ -1494,126 +1404,6 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>75.5</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>62.5</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>59.5</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>57.5</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>55.5</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>54.5</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>53.5</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>53.5</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>53.5</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>52.5</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>52.5</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>49.5</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>49.5</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>48.5</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>49.5</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>49.5</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1653,10 +1443,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$110</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>42695.855162037034</c:v>
                 </c:pt>
@@ -1959,136 +1749,16 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>42695.866736111115</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>42695.866851851853</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>42695.866967592592</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>42695.867083333331</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>42695.867199074077</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>42695.867314814815</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>42695.867430555554</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>42695.867546296293</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>42695.867662037039</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>42695.867777777778</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>42695.867893518516</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>42695.868009259262</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>42695.868125000001</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>42695.86824074074</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>42695.868356481478</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>42695.868472222224</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>42695.868587962963</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>42695.868703703702</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>42695.868819444448</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>42695.868935185186</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>42695.869050925925</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>42695.869166666664</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>42695.86928240741</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>42695.869398148148</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>42695.869513888887</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>42695.869629629633</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>42695.869745370372</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>42695.86986111111</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>42695.869976851849</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>42695.870092592595</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>42695.870208333334</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>42695.870324074072</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>42695.870439814818</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>42695.870555555557</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>42695.870671296296</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>42695.870787037034</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>42695.87090277778</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>42695.871018518519</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>42695.871134259258</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>42695.871249999997</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>42695.871365740742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$R$10:$R$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$R$10:$R$110</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>58.5</c:v>
                 </c:pt>
@@ -2390,126 +2060,6 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="140">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2550,10 +2100,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$T$10:$T$110</c:f>
               <c:numCache>
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>42695.855162037034</c:v>
                 </c:pt>
@@ -2856,136 +2406,16 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>42695.866736111115</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>42695.866851851853</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>42695.866967592592</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>42695.867083333331</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>42695.867199074077</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>42695.867314814815</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>42695.867430555554</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>42695.867546296293</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>42695.867662037039</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>42695.867777777778</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>42695.867893518516</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>42695.868009259262</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>42695.868125000001</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>42695.86824074074</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>42695.868356481478</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>42695.868472222224</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>42695.868587962963</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>42695.868703703702</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>42695.868819444448</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>42695.868935185186</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>42695.869050925925</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>42695.869166666664</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>42695.86928240741</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>42695.869398148148</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>42695.869513888887</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>42695.869629629633</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>42695.869745370372</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>42695.86986111111</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>42695.869976851849</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>42695.870092592595</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>42695.870208333334</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>42695.870324074072</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>42695.870439814818</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>42695.870555555557</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>42695.870671296296</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>42695.870787037034</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>42695.87090277778</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>42695.871018518519</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>42695.871134259258</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>42695.871249999997</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>42695.871365740742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CT-Log 2016-11-21 20-31-16'!$S$10:$S$150</c:f>
+              <c:f>'CT-Log 2016-11-21 20-31-16'!$S$10:$S$110</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="141"/>
+                <c:ptCount val="101"/>
                 <c:pt idx="0">
                   <c:v>24.2</c:v>
                 </c:pt>
@@ -3288,126 +2718,6 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>8.1</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>7.9</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>7.8</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>7.7</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7.4</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>7.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4187,7 +3497,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4504,17 +3820,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4534,14 +3850,14 @@
         <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N1">
         <f xml:space="preserve"> K4/K7</f>
         <v>588150.6626876673</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4561,7 +3877,7 @@
         <v>2048000000</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4585,7 +3901,7 @@
         <v>16384000000</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4609,7 +3925,7 @@
         <v>16950755.066685535</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4626,14 +3942,14 @@
         <v>918.96095078829603</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5">
         <f>K4/1000000</f>
         <v>16.950755066685534</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G6">
         <f>SUM(G2:G5)</f>
         <v>8</v>
@@ -4643,7 +3959,7 @@
         <v>966.564612345829</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4651,14 +3967,14 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7">
         <f>AVERAGE(S10:S102)</f>
         <v>28.820430107526885</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4717,7 +4033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>42695.855162037034</v>
       </c>
@@ -4771,7 +4087,7 @@
         <v>42695.855162037034</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>42695.85527777778</v>
       </c>
@@ -4825,7 +4141,7 @@
         <v>42695.85527777778</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>42695.855393518519</v>
       </c>
@@ -4879,7 +4195,7 @@
         <v>42695.855393518519</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>42695.855509259258</v>
       </c>
@@ -4933,7 +4249,7 @@
         <v>42695.855509259258</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>42695.855624999997</v>
       </c>
@@ -4987,7 +4303,7 @@
         <v>42695.855624999997</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>42695.855740740742</v>
       </c>
@@ -5041,7 +4357,7 @@
         <v>42695.855740740742</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>42695.855856481481</v>
       </c>
@@ -5095,7 +4411,7 @@
         <v>42695.855856481481</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>42695.85597222222</v>
       </c>
@@ -5149,7 +4465,7 @@
         <v>42695.85597222222</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>42695.856087962966</v>
       </c>
@@ -5203,7 +4519,7 @@
         <v>42695.856087962966</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>42695.856203703705</v>
       </c>
@@ -5257,7 +4573,7 @@
         <v>42695.856203703705</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>42695.856319444443</v>
       </c>
@@ -5311,7 +4627,7 @@
         <v>42695.856319444443</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>42695.856435185182</v>
       </c>
@@ -5365,7 +4681,7 @@
         <v>42695.856435185182</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42695.856550925928</v>
       </c>
@@ -5419,7 +4735,7 @@
         <v>42695.856550925928</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42695.856666666667</v>
       </c>
@@ -5473,7 +4789,7 @@
         <v>42695.856666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42695.856782407405</v>
       </c>
@@ -5527,7 +4843,7 @@
         <v>42695.856782407405</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>42695.856898148151</v>
       </c>
@@ -5581,7 +4897,7 @@
         <v>42695.856898148151</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>42695.85701388889</v>
       </c>
@@ -5635,7 +4951,7 @@
         <v>42695.85701388889</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>42695.857129629629</v>
       </c>
@@ -5689,7 +5005,7 @@
         <v>42695.857129629629</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>42695.857245370367</v>
       </c>
@@ -5743,7 +5059,7 @@
         <v>42695.857245370367</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>42695.857361111113</v>
       </c>
@@ -5797,7 +5113,7 @@
         <v>42695.857361111113</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>42695.857476851852</v>
       </c>
@@ -5851,7 +5167,7 @@
         <v>42695.857476851852</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>42695.857592592591</v>
       </c>
@@ -5905,7 +5221,7 @@
         <v>42695.857592592591</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>42695.857708333337</v>
       </c>
@@ -5959,7 +5275,7 @@
         <v>42695.857708333337</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>42695.857824074075</v>
       </c>
@@ -6013,7 +5329,7 @@
         <v>42695.857824074075</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>42695.857939814814</v>
       </c>
@@ -6067,7 +5383,7 @@
         <v>42695.857939814814</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>42695.858055555553</v>
       </c>
@@ -6121,7 +5437,7 @@
         <v>42695.858055555553</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>42695.858171296299</v>
       </c>
@@ -6175,7 +5491,7 @@
         <v>42695.858171296299</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>42695.858287037037</v>
       </c>
@@ -6229,7 +5545,7 @@
         <v>42695.858287037037</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>42695.858402777776</v>
       </c>
@@ -6283,7 +5599,7 @@
         <v>42695.858402777776</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>42695.858518518522</v>
       </c>
@@ -6337,7 +5653,7 @@
         <v>42695.858518518522</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>42695.858634259261</v>
       </c>
@@ -6391,7 +5707,7 @@
         <v>42695.858634259261</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>42695.858749999999</v>
       </c>
@@ -6445,7 +5761,7 @@
         <v>42695.858749999999</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42695.858865740738</v>
       </c>
@@ -6499,7 +5815,7 @@
         <v>42695.858865740738</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42695.858981481484</v>
       </c>
@@ -6553,7 +5869,7 @@
         <v>42695.858981481484</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42695.859097222223</v>
       </c>
@@ -6607,7 +5923,7 @@
         <v>42695.859097222223</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>42695.859212962961</v>
       </c>
@@ -6661,7 +5977,7 @@
         <v>42695.859212962961</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>42695.8593287037</v>
       </c>
@@ -6715,7 +6031,7 @@
         <v>42695.8593287037</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>42695.859444444446</v>
       </c>
@@ -6769,7 +6085,7 @@
         <v>42695.859444444446</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>42695.859560185185</v>
       </c>
@@ -6823,7 +6139,7 @@
         <v>42695.859560185185</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>42695.859675925924</v>
       </c>
@@ -6877,7 +6193,7 @@
         <v>42695.859675925924</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>42695.859791666669</v>
       </c>
@@ -6931,7 +6247,7 @@
         <v>42695.859791666669</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>42695.859907407408</v>
       </c>
@@ -6985,7 +6301,7 @@
         <v>42695.859907407408</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>42695.860023148147</v>
       </c>
@@ -7039,7 +6355,7 @@
         <v>42695.860023148147</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>42695.860138888886</v>
       </c>
@@ -7093,7 +6409,7 @@
         <v>42695.860138888886</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>42695.860254629632</v>
       </c>
@@ -7147,7 +6463,7 @@
         <v>42695.860254629632</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>42695.86037037037</v>
       </c>
@@ -7201,7 +6517,7 @@
         <v>42695.86037037037</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>42695.860486111109</v>
       </c>
@@ -7255,7 +6571,7 @@
         <v>42695.860486111109</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>42695.860601851855</v>
       </c>
@@ -7309,7 +6625,7 @@
         <v>42695.860601851855</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>42695.860717592594</v>
       </c>
@@ -7363,7 +6679,7 @@
         <v>42695.860717592594</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>42695.860833333332</v>
       </c>
@@ -7417,7 +6733,7 @@
         <v>42695.860833333332</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>42695.860949074071</v>
       </c>
@@ -7471,7 +6787,7 @@
         <v>42695.860949074071</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>42695.861064814817</v>
       </c>
@@ -7525,7 +6841,7 @@
         <v>42695.861064814817</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>42695.861180555556</v>
       </c>
@@ -7579,7 +6895,7 @@
         <v>42695.861180555556</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>42695.861296296294</v>
       </c>
@@ -7633,7 +6949,7 @@
         <v>42695.861296296294</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>42695.86141203704</v>
       </c>
@@ -7687,7 +7003,7 @@
         <v>42695.86141203704</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>42695.861527777779</v>
       </c>
@@ -7741,7 +7057,7 @@
         <v>42695.861527777779</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>42695.861643518518</v>
       </c>
@@ -7795,7 +7111,7 @@
         <v>42695.861643518518</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>42695.861759259256</v>
       </c>
@@ -7849,7 +7165,7 @@
         <v>42695.861759259256</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>42695.861875000002</v>
       </c>
@@ -7903,7 +7219,7 @@
         <v>42695.861875000002</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>42695.861990740741</v>
       </c>
@@ -7957,7 +7273,7 @@
         <v>42695.861990740741</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>42695.86210648148</v>
       </c>
@@ -8011,7 +7327,7 @@
         <v>42695.86210648148</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>42695.862222222226</v>
       </c>
@@ -8065,7 +7381,7 @@
         <v>42695.862222222226</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>42695.862337962964</v>
       </c>
@@ -8119,7 +7435,7 @@
         <v>42695.862337962964</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>42695.862453703703</v>
       </c>
@@ -8173,7 +7489,7 @@
         <v>42695.862453703703</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>42695.862569444442</v>
       </c>
@@ -8227,7 +7543,7 @@
         <v>42695.862569444442</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>42695.862685185188</v>
       </c>
@@ -8281,7 +7597,7 @@
         <v>42695.862685185188</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>42695.862800925926</v>
       </c>
@@ -8335,7 +7651,7 @@
         <v>42695.862800925926</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>42695.862916666665</v>
       </c>
@@ -8389,7 +7705,7 @@
         <v>42695.862916666665</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>42695.863032407404</v>
       </c>
@@ -8443,7 +7759,7 @@
         <v>42695.863032407404</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>42695.86314814815</v>
       </c>
@@ -8497,7 +7813,7 @@
         <v>42695.86314814815</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>42695.863263888888</v>
       </c>
@@ -8551,7 +7867,7 @@
         <v>42695.863263888888</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>42695.863379629627</v>
       </c>
@@ -8605,7 +7921,7 @@
         <v>42695.863379629627</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>42695.863495370373</v>
       </c>
@@ -8659,7 +7975,7 @@
         <v>42695.863495370373</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>42695.863611111112</v>
       </c>
@@ -8713,7 +8029,7 @@
         <v>42695.863611111112</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>42695.863726851851</v>
       </c>
@@ -8767,7 +8083,7 @@
         <v>42695.863726851851</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>42695.863842592589</v>
       </c>
@@ -8821,7 +8137,7 @@
         <v>42695.863842592589</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>42695.863958333335</v>
       </c>
@@ -8875,7 +8191,7 @@
         <v>42695.863958333335</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>42695.864074074074</v>
       </c>
@@ -8929,7 +8245,7 @@
         <v>42695.864074074074</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>42695.864189814813</v>
       </c>
@@ -8983,7 +8299,7 @@
         <v>42695.864189814813</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>42695.864305555559</v>
       </c>
@@ -9037,7 +8353,7 @@
         <v>42695.864305555559</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>42695.864421296297</v>
       </c>
@@ -9091,7 +8407,7 @@
         <v>42695.864421296297</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>42695.864537037036</v>
       </c>
@@ -9145,7 +8461,7 @@
         <v>42695.864537037036</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>42695.864652777775</v>
       </c>
@@ -9199,7 +8515,7 @@
         <v>42695.864652777775</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>42695.864768518521</v>
       </c>
@@ -9253,7 +8569,7 @@
         <v>42695.864768518521</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>42695.864884259259</v>
       </c>
@@ -9307,7 +8623,7 @@
         <v>42695.864884259259</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>42695.864999999998</v>
       </c>
@@ -9361,7 +8677,7 @@
         <v>42695.864999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>42695.865115740744</v>
       </c>
@@ -9415,7 +8731,7 @@
         <v>42695.865115740744</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>42695.865231481483</v>
       </c>
@@ -9469,7 +8785,7 @@
         <v>42695.865231481483</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>42695.865347222221</v>
       </c>
@@ -9523,7 +8839,7 @@
         <v>42695.865347222221</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>42695.86546296296</v>
       </c>
@@ -9577,7 +8893,7 @@
         <v>42695.86546296296</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>42695.865578703706</v>
       </c>
@@ -9631,7 +8947,7 @@
         <v>42695.865578703706</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>42695.865694444445</v>
       </c>
@@ -9685,7 +9001,7 @@
         <v>42695.865694444445</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>42695.865810185183</v>
       </c>
@@ -9739,7 +9055,7 @@
         <v>42695.865810185183</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>42695.865925925929</v>
       </c>
@@ -9793,7 +9109,7 @@
         <v>42695.865925925929</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>42695.866041666668</v>
       </c>
@@ -9847,7 +9163,7 @@
         <v>42695.866041666668</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>42695.866157407407</v>
       </c>
@@ -9901,7 +9217,7 @@
         <v>42695.866157407407</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>42695.866273148145</v>
       </c>
@@ -9955,7 +9271,7 @@
         <v>42695.866273148145</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>42695.866388888891</v>
       </c>
@@ -10009,7 +9325,7 @@
         <v>42695.866388888891</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>42695.86650462963</v>
       </c>
@@ -10063,7 +9379,7 @@
         <v>42695.86650462963</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>42695.866620370369</v>
       </c>
@@ -10117,7 +9433,7 @@
         <v>42695.866620370369</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>42695.866736111115</v>
       </c>
@@ -10171,2467 +9487,467 @@
         <v>42695.866736111115</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>42695.866851851853</v>
-      </c>
-      <c r="B111">
-        <v>73</v>
-      </c>
-      <c r="C111">
-        <v>73</v>
-      </c>
-      <c r="F111">
-        <v>52</v>
-      </c>
-      <c r="G111">
-        <v>105</v>
-      </c>
-      <c r="H111">
-        <v>1</v>
-      </c>
-      <c r="I111">
-        <v>3292.64</v>
-      </c>
-      <c r="K111">
-        <v>49</v>
-      </c>
-      <c r="L111">
-        <v>103</v>
-      </c>
-      <c r="M111">
-        <v>0</v>
-      </c>
-      <c r="N111">
-        <v>3292.64</v>
-      </c>
-      <c r="O111">
-        <v>7.8</v>
-      </c>
-      <c r="Q111">
-        <f t="shared" si="4"/>
-        <v>73</v>
-      </c>
-      <c r="R111">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S111">
-        <f t="shared" si="6"/>
-        <v>7.8</v>
-      </c>
-      <c r="T111" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.866851851853</v>
-      </c>
-    </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>42695.866967592592</v>
-      </c>
-      <c r="B112">
-        <v>72</v>
-      </c>
-      <c r="C112">
-        <v>71</v>
-      </c>
-      <c r="F112">
-        <v>52</v>
-      </c>
-      <c r="G112">
-        <v>105</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
-      <c r="I112">
-        <v>3292.64</v>
-      </c>
-      <c r="K112">
-        <v>49</v>
-      </c>
-      <c r="L112">
-        <v>103</v>
-      </c>
-      <c r="M112">
-        <v>0</v>
-      </c>
-      <c r="N112">
-        <v>3292.64</v>
-      </c>
-      <c r="O112">
-        <v>8.1</v>
-      </c>
-      <c r="Q112">
-        <f t="shared" si="4"/>
-        <v>71.5</v>
-      </c>
-      <c r="R112">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S112">
-        <f t="shared" si="6"/>
-        <v>8.1</v>
-      </c>
-      <c r="T112" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.866967592592</v>
-      </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>42695.867083333331</v>
-      </c>
-      <c r="B113">
-        <v>70</v>
-      </c>
-      <c r="C113">
-        <v>72</v>
-      </c>
-      <c r="F113">
-        <v>52</v>
-      </c>
-      <c r="G113">
-        <v>105</v>
-      </c>
-      <c r="H113">
-        <v>0</v>
-      </c>
-      <c r="I113">
-        <v>3292.64</v>
-      </c>
-      <c r="K113">
-        <v>49</v>
-      </c>
-      <c r="L113">
-        <v>103</v>
-      </c>
-      <c r="M113">
-        <v>0</v>
-      </c>
-      <c r="N113">
-        <v>3292.64</v>
-      </c>
-      <c r="O113">
-        <v>7.8</v>
-      </c>
-      <c r="Q113">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="R113">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S113">
-        <f t="shared" si="6"/>
-        <v>7.8</v>
-      </c>
-      <c r="T113" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867083333331</v>
-      </c>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>42695.867199074077</v>
-      </c>
-      <c r="B114">
-        <v>69</v>
-      </c>
-      <c r="C114">
-        <v>69</v>
-      </c>
-      <c r="F114">
-        <v>52</v>
-      </c>
-      <c r="G114">
-        <v>105</v>
-      </c>
-      <c r="H114">
-        <v>1</v>
-      </c>
-      <c r="I114">
-        <v>3292.64</v>
-      </c>
-      <c r="K114">
-        <v>49</v>
-      </c>
-      <c r="L114">
-        <v>103</v>
-      </c>
-      <c r="M114">
-        <v>1</v>
-      </c>
-      <c r="N114">
-        <v>3292.64</v>
-      </c>
-      <c r="O114">
-        <v>7.8</v>
-      </c>
-      <c r="Q114">
-        <f t="shared" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="R114">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S114">
-        <f t="shared" si="6"/>
-        <v>7.8</v>
-      </c>
-      <c r="T114" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867199074077</v>
-      </c>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>42695.867314814815</v>
-      </c>
-      <c r="B115">
-        <v>69</v>
-      </c>
-      <c r="C115">
-        <v>69</v>
-      </c>
-      <c r="F115">
-        <v>52</v>
-      </c>
-      <c r="G115">
-        <v>105</v>
-      </c>
-      <c r="H115">
-        <v>2</v>
-      </c>
-      <c r="I115">
-        <v>3292.64</v>
-      </c>
-      <c r="K115">
-        <v>49</v>
-      </c>
-      <c r="L115">
-        <v>103</v>
-      </c>
-      <c r="M115">
-        <v>0</v>
-      </c>
-      <c r="N115">
-        <v>3292.64</v>
-      </c>
-      <c r="O115">
-        <v>7.9</v>
-      </c>
-      <c r="Q115">
-        <f t="shared" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="R115">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S115">
-        <f t="shared" si="6"/>
-        <v>7.9</v>
-      </c>
-      <c r="T115" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867314814815</v>
-      </c>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>42695.867430555554</v>
-      </c>
-      <c r="B116">
-        <v>67</v>
-      </c>
-      <c r="C116">
-        <v>67</v>
-      </c>
-      <c r="F116">
-        <v>52</v>
-      </c>
-      <c r="G116">
-        <v>105</v>
-      </c>
-      <c r="H116">
-        <v>1</v>
-      </c>
-      <c r="I116">
-        <v>3292.64</v>
-      </c>
-      <c r="K116">
-        <v>49</v>
-      </c>
-      <c r="L116">
-        <v>103</v>
-      </c>
-      <c r="M116">
-        <v>0</v>
-      </c>
-      <c r="N116">
-        <v>3292.64</v>
-      </c>
-      <c r="O116">
-        <v>7.7</v>
-      </c>
-      <c r="Q116">
-        <f t="shared" si="4"/>
-        <v>67</v>
-      </c>
-      <c r="R116">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S116">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T116" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867430555554</v>
-      </c>
-    </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>42695.867546296293</v>
-      </c>
-      <c r="B117">
-        <v>66</v>
-      </c>
-      <c r="C117">
-        <v>66</v>
-      </c>
-      <c r="F117">
-        <v>52</v>
-      </c>
-      <c r="G117">
-        <v>105</v>
-      </c>
-      <c r="H117">
-        <v>1</v>
-      </c>
-      <c r="I117">
-        <v>3292.64</v>
-      </c>
-      <c r="K117">
-        <v>49</v>
-      </c>
-      <c r="L117">
-        <v>103</v>
-      </c>
-      <c r="M117">
-        <v>0</v>
-      </c>
-      <c r="N117">
-        <v>3292.64</v>
-      </c>
-      <c r="O117">
-        <v>7.7</v>
-      </c>
-      <c r="Q117">
-        <f t="shared" si="4"/>
-        <v>66</v>
-      </c>
-      <c r="R117">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S117">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T117" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867546296293</v>
-      </c>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>42695.867662037039</v>
-      </c>
-      <c r="B118">
-        <v>64</v>
-      </c>
-      <c r="C118">
-        <v>64</v>
-      </c>
-      <c r="F118">
-        <v>52</v>
-      </c>
-      <c r="G118">
-        <v>105</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118">
-        <v>3292.64</v>
-      </c>
-      <c r="K118">
-        <v>49</v>
-      </c>
-      <c r="L118">
-        <v>103</v>
-      </c>
-      <c r="M118">
-        <v>0</v>
-      </c>
-      <c r="N118">
-        <v>3292.64</v>
-      </c>
-      <c r="O118">
-        <v>7.8</v>
-      </c>
-      <c r="Q118">
-        <f t="shared" si="4"/>
-        <v>64</v>
-      </c>
-      <c r="R118">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S118">
-        <f t="shared" si="6"/>
-        <v>7.8</v>
-      </c>
-      <c r="T118" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867662037039</v>
-      </c>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>42695.867777777778</v>
-      </c>
-      <c r="B119">
-        <v>64</v>
-      </c>
-      <c r="C119">
-        <v>64</v>
-      </c>
-      <c r="F119">
-        <v>52</v>
-      </c>
-      <c r="G119">
-        <v>105</v>
-      </c>
-      <c r="H119">
-        <v>1</v>
-      </c>
-      <c r="I119">
-        <v>3292.64</v>
-      </c>
-      <c r="K119">
-        <v>49</v>
-      </c>
-      <c r="L119">
-        <v>103</v>
-      </c>
-      <c r="M119">
-        <v>0</v>
-      </c>
-      <c r="N119">
-        <v>3292.64</v>
-      </c>
-      <c r="O119">
-        <v>7.7</v>
-      </c>
-      <c r="Q119">
-        <f t="shared" si="4"/>
-        <v>64</v>
-      </c>
-      <c r="R119">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S119">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T119" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867777777778</v>
-      </c>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>42695.867893518516</v>
-      </c>
-      <c r="B120">
-        <v>63</v>
-      </c>
-      <c r="C120">
-        <v>63</v>
-      </c>
-      <c r="F120">
-        <v>52</v>
-      </c>
-      <c r="G120">
-        <v>105</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120">
-        <v>3292.64</v>
-      </c>
-      <c r="K120">
-        <v>49</v>
-      </c>
-      <c r="L120">
-        <v>103</v>
-      </c>
-      <c r="M120">
-        <v>0</v>
-      </c>
-      <c r="N120">
-        <v>3292.64</v>
-      </c>
-      <c r="O120">
-        <v>7.7</v>
-      </c>
-      <c r="Q120">
-        <f t="shared" si="4"/>
-        <v>63</v>
-      </c>
-      <c r="R120">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S120">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T120" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.867893518516</v>
-      </c>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>42695.868009259262</v>
-      </c>
-      <c r="B121">
-        <v>63</v>
-      </c>
-      <c r="C121">
-        <v>62</v>
-      </c>
-      <c r="F121">
-        <v>52</v>
-      </c>
-      <c r="G121">
-        <v>105</v>
-      </c>
-      <c r="H121">
-        <v>1</v>
-      </c>
-      <c r="I121">
-        <v>3292.64</v>
-      </c>
-      <c r="K121">
-        <v>49</v>
-      </c>
-      <c r="L121">
-        <v>103</v>
-      </c>
-      <c r="M121">
-        <v>0</v>
-      </c>
-      <c r="N121">
-        <v>3292.64</v>
-      </c>
-      <c r="O121">
-        <v>7.7</v>
-      </c>
-      <c r="Q121">
-        <f t="shared" si="4"/>
-        <v>62.5</v>
-      </c>
-      <c r="R121">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S121">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T121" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868009259262</v>
-      </c>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>42695.868125000001</v>
-      </c>
-      <c r="B122">
-        <v>62</v>
-      </c>
-      <c r="C122">
-        <v>60</v>
-      </c>
-      <c r="F122">
-        <v>52</v>
-      </c>
-      <c r="G122">
-        <v>105</v>
-      </c>
-      <c r="H122">
-        <v>1</v>
-      </c>
-      <c r="I122">
-        <v>3292.64</v>
-      </c>
-      <c r="K122">
-        <v>49</v>
-      </c>
-      <c r="L122">
-        <v>103</v>
-      </c>
-      <c r="M122">
-        <v>0</v>
-      </c>
-      <c r="N122">
-        <v>3292.64</v>
-      </c>
-      <c r="O122">
-        <v>7.6</v>
-      </c>
-      <c r="Q122">
-        <f t="shared" si="4"/>
-        <v>61</v>
-      </c>
-      <c r="R122">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S122">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T122" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868125000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>42695.86824074074</v>
-      </c>
-      <c r="B123">
-        <v>61</v>
-      </c>
-      <c r="C123">
-        <v>61</v>
-      </c>
-      <c r="F123">
-        <v>52</v>
-      </c>
-      <c r="G123">
-        <v>105</v>
-      </c>
-      <c r="H123">
-        <v>0</v>
-      </c>
-      <c r="I123">
-        <v>3292.64</v>
-      </c>
-      <c r="K123">
-        <v>49</v>
-      </c>
-      <c r="L123">
-        <v>103</v>
-      </c>
-      <c r="M123">
-        <v>0</v>
-      </c>
-      <c r="N123">
-        <v>3292.64</v>
-      </c>
-      <c r="O123">
-        <v>7.7</v>
-      </c>
-      <c r="Q123">
-        <f t="shared" si="4"/>
-        <v>61</v>
-      </c>
-      <c r="R123">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S123">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T123" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.86824074074</v>
-      </c>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>42695.868356481478</v>
-      </c>
-      <c r="B124">
-        <v>61</v>
-      </c>
-      <c r="C124">
-        <v>59</v>
-      </c>
-      <c r="F124">
-        <v>52</v>
-      </c>
-      <c r="G124">
-        <v>105</v>
-      </c>
-      <c r="H124">
-        <v>0</v>
-      </c>
-      <c r="I124">
-        <v>3292.64</v>
-      </c>
-      <c r="K124">
-        <v>49</v>
-      </c>
-      <c r="L124">
-        <v>103</v>
-      </c>
-      <c r="M124">
-        <v>0</v>
-      </c>
-      <c r="N124">
-        <v>3292.64</v>
-      </c>
-      <c r="O124">
-        <v>7.7</v>
-      </c>
-      <c r="Q124">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="R124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S124">
-        <f t="shared" si="6"/>
-        <v>7.7</v>
-      </c>
-      <c r="T124" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868356481478</v>
-      </c>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>42695.868472222224</v>
-      </c>
-      <c r="B125">
-        <v>60</v>
-      </c>
-      <c r="C125">
-        <v>58</v>
-      </c>
-      <c r="F125">
-        <v>52</v>
-      </c>
-      <c r="G125">
-        <v>105</v>
-      </c>
-      <c r="H125">
-        <v>0</v>
-      </c>
-      <c r="I125">
-        <v>3292.64</v>
-      </c>
-      <c r="K125">
-        <v>49</v>
-      </c>
-      <c r="L125">
-        <v>103</v>
-      </c>
-      <c r="M125">
-        <v>0</v>
-      </c>
-      <c r="N125">
-        <v>3292.64</v>
-      </c>
-      <c r="O125">
-        <v>7.6</v>
-      </c>
-      <c r="Q125">
-        <f t="shared" si="4"/>
-        <v>59</v>
-      </c>
-      <c r="R125">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S125">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T125" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868472222224</v>
-      </c>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>42695.868587962963</v>
-      </c>
-      <c r="B126">
-        <v>60</v>
-      </c>
-      <c r="C126">
-        <v>59</v>
-      </c>
-      <c r="F126">
-        <v>52</v>
-      </c>
-      <c r="G126">
-        <v>105</v>
-      </c>
-      <c r="H126">
-        <v>1</v>
-      </c>
-      <c r="I126">
-        <v>3292.64</v>
-      </c>
-      <c r="K126">
-        <v>49</v>
-      </c>
-      <c r="L126">
-        <v>103</v>
-      </c>
-      <c r="M126">
-        <v>0</v>
-      </c>
-      <c r="N126">
-        <v>3292.64</v>
-      </c>
-      <c r="O126">
-        <v>7.4</v>
-      </c>
-      <c r="Q126">
-        <f t="shared" si="4"/>
-        <v>59.5</v>
-      </c>
-      <c r="R126">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S126">
-        <f t="shared" si="6"/>
-        <v>7.4</v>
-      </c>
-      <c r="T126" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868587962963</v>
-      </c>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>42695.868703703702</v>
-      </c>
-      <c r="B127">
-        <v>58</v>
-      </c>
-      <c r="C127">
-        <v>57</v>
-      </c>
-      <c r="F127">
-        <v>52</v>
-      </c>
-      <c r="G127">
-        <v>105</v>
-      </c>
-      <c r="H127">
-        <v>0</v>
-      </c>
-      <c r="I127">
-        <v>3292.64</v>
-      </c>
-      <c r="K127">
-        <v>49</v>
-      </c>
-      <c r="L127">
-        <v>103</v>
-      </c>
-      <c r="M127">
-        <v>0</v>
-      </c>
-      <c r="N127">
-        <v>3292.64</v>
-      </c>
-      <c r="O127">
-        <v>7.6</v>
-      </c>
-      <c r="Q127">
-        <f t="shared" si="4"/>
-        <v>57.5</v>
-      </c>
-      <c r="R127">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S127">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T127" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868703703702</v>
-      </c>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>42695.868819444448</v>
-      </c>
-      <c r="B128">
-        <v>57</v>
-      </c>
-      <c r="C128">
-        <v>57</v>
-      </c>
-      <c r="F128">
-        <v>52</v>
-      </c>
-      <c r="G128">
-        <v>105</v>
-      </c>
-      <c r="H128">
-        <v>1</v>
-      </c>
-      <c r="I128">
-        <v>3292.64</v>
-      </c>
-      <c r="K128">
-        <v>49</v>
-      </c>
-      <c r="L128">
-        <v>103</v>
-      </c>
-      <c r="M128">
-        <v>0</v>
-      </c>
-      <c r="N128">
-        <v>3292.64</v>
-      </c>
-      <c r="O128">
-        <v>7.5</v>
-      </c>
-      <c r="Q128">
-        <f t="shared" si="4"/>
-        <v>57</v>
-      </c>
-      <c r="R128">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S128">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="T128" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868819444448</v>
-      </c>
-    </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>42695.868935185186</v>
-      </c>
-      <c r="B129">
-        <v>57</v>
-      </c>
-      <c r="C129">
-        <v>57</v>
-      </c>
-      <c r="F129">
-        <v>52</v>
-      </c>
-      <c r="G129">
-        <v>105</v>
-      </c>
-      <c r="H129">
-        <v>1</v>
-      </c>
-      <c r="I129">
-        <v>3292.64</v>
-      </c>
-      <c r="K129">
-        <v>49</v>
-      </c>
-      <c r="L129">
-        <v>103</v>
-      </c>
-      <c r="M129">
-        <v>0</v>
-      </c>
-      <c r="N129">
-        <v>3292.64</v>
-      </c>
-      <c r="O129">
-        <v>7.5</v>
-      </c>
-      <c r="Q129">
-        <f t="shared" si="4"/>
-        <v>57</v>
-      </c>
-      <c r="R129">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S129">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="T129" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.868935185186</v>
-      </c>
-    </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>42695.869050925925</v>
-      </c>
-      <c r="B130">
-        <v>59</v>
-      </c>
-      <c r="C130">
-        <v>57</v>
-      </c>
-      <c r="F130">
-        <v>52</v>
-      </c>
-      <c r="G130">
-        <v>105</v>
-      </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-      <c r="I130">
-        <v>3292.64</v>
-      </c>
-      <c r="K130">
-        <v>49</v>
-      </c>
-      <c r="L130">
-        <v>103</v>
-      </c>
-      <c r="M130">
-        <v>0</v>
-      </c>
-      <c r="N130">
-        <v>3292.64</v>
-      </c>
-      <c r="O130">
-        <v>7.6</v>
-      </c>
-      <c r="Q130">
-        <f t="shared" si="4"/>
-        <v>58</v>
-      </c>
-      <c r="R130">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S130">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T130" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869050925925</v>
-      </c>
-    </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>42695.869166666664</v>
-      </c>
-      <c r="B131">
-        <v>55</v>
-      </c>
-      <c r="C131">
-        <v>56</v>
-      </c>
-      <c r="F131">
-        <v>52</v>
-      </c>
-      <c r="G131">
-        <v>105</v>
-      </c>
-      <c r="H131">
-        <v>1</v>
-      </c>
-      <c r="I131">
-        <v>3292.64</v>
-      </c>
-      <c r="K131">
-        <v>49</v>
-      </c>
-      <c r="L131">
-        <v>103</v>
-      </c>
-      <c r="M131">
-        <v>1</v>
-      </c>
-      <c r="N131">
-        <v>3292.64</v>
-      </c>
-      <c r="O131">
-        <v>7.6</v>
-      </c>
-      <c r="Q131">
-        <f t="shared" si="4"/>
-        <v>55.5</v>
-      </c>
-      <c r="R131">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S131">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T131" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869166666664</v>
-      </c>
-    </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>42695.86928240741</v>
-      </c>
-      <c r="B132">
-        <v>55</v>
-      </c>
-      <c r="C132">
-        <v>54</v>
-      </c>
-      <c r="F132">
-        <v>52</v>
-      </c>
-      <c r="G132">
-        <v>105</v>
-      </c>
-      <c r="H132">
-        <v>1</v>
-      </c>
-      <c r="I132">
-        <v>3292.64</v>
-      </c>
-      <c r="K132">
-        <v>49</v>
-      </c>
-      <c r="L132">
-        <v>103</v>
-      </c>
-      <c r="M132">
-        <v>1</v>
-      </c>
-      <c r="N132">
-        <v>3292.64</v>
-      </c>
-      <c r="O132">
-        <v>7.5</v>
-      </c>
-      <c r="Q132">
-        <f t="shared" si="4"/>
-        <v>54.5</v>
-      </c>
-      <c r="R132">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="S132">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="T132" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.86928240741</v>
-      </c>
-    </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>42695.869398148148</v>
-      </c>
-      <c r="B133">
-        <v>56</v>
-      </c>
-      <c r="C133">
-        <v>54</v>
-      </c>
-      <c r="F133">
-        <v>52</v>
-      </c>
-      <c r="G133">
-        <v>105</v>
-      </c>
-      <c r="H133">
-        <v>1</v>
-      </c>
-      <c r="I133">
-        <v>3292.64</v>
-      </c>
-      <c r="K133">
-        <v>49</v>
-      </c>
-      <c r="L133">
-        <v>103</v>
-      </c>
-      <c r="M133">
-        <v>0</v>
-      </c>
-      <c r="N133">
-        <v>3292.64</v>
-      </c>
-      <c r="O133">
-        <v>7.5</v>
-      </c>
-      <c r="Q133">
-        <f t="shared" si="4"/>
-        <v>55</v>
-      </c>
-      <c r="R133">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S133">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="T133" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869398148148</v>
-      </c>
-    </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>42695.869513888887</v>
-      </c>
-      <c r="B134">
-        <v>54</v>
-      </c>
-      <c r="C134">
-        <v>53</v>
-      </c>
-      <c r="F134">
-        <v>52</v>
-      </c>
-      <c r="G134">
-        <v>105</v>
-      </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-      <c r="I134">
-        <v>3292.64</v>
-      </c>
-      <c r="K134">
-        <v>49</v>
-      </c>
-      <c r="L134">
-        <v>103</v>
-      </c>
-      <c r="M134">
-        <v>0</v>
-      </c>
-      <c r="N134">
-        <v>3292.64</v>
-      </c>
-      <c r="O134">
-        <v>7.6</v>
-      </c>
-      <c r="Q134">
-        <f t="shared" si="4"/>
-        <v>53.5</v>
-      </c>
-      <c r="R134">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S134">
-        <f t="shared" si="6"/>
-        <v>7.6</v>
-      </c>
-      <c r="T134" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869513888887</v>
-      </c>
-    </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>42695.869629629633</v>
-      </c>
-      <c r="B135">
-        <v>55</v>
-      </c>
-      <c r="C135">
-        <v>52</v>
-      </c>
-      <c r="F135">
-        <v>52</v>
-      </c>
-      <c r="G135">
-        <v>105</v>
-      </c>
-      <c r="H135">
-        <v>0</v>
-      </c>
-      <c r="I135">
-        <v>3292.64</v>
-      </c>
-      <c r="K135">
-        <v>49</v>
-      </c>
-      <c r="L135">
-        <v>103</v>
-      </c>
-      <c r="M135">
-        <v>0</v>
-      </c>
-      <c r="N135">
-        <v>3292.64</v>
-      </c>
-      <c r="O135">
-        <v>7.4</v>
-      </c>
-      <c r="Q135">
-        <f t="shared" si="4"/>
-        <v>53.5</v>
-      </c>
-      <c r="R135">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S135">
-        <f t="shared" si="6"/>
-        <v>7.4</v>
-      </c>
-      <c r="T135" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869629629633</v>
-      </c>
-    </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
-        <v>42695.869745370372</v>
-      </c>
-      <c r="B136">
-        <v>54</v>
-      </c>
-      <c r="C136">
-        <v>53</v>
-      </c>
-      <c r="F136">
-        <v>52</v>
-      </c>
-      <c r="G136">
-        <v>105</v>
-      </c>
-      <c r="H136">
-        <v>0</v>
-      </c>
-      <c r="I136">
-        <v>3292.64</v>
-      </c>
-      <c r="K136">
-        <v>49</v>
-      </c>
-      <c r="L136">
-        <v>103</v>
-      </c>
-      <c r="M136">
-        <v>0</v>
-      </c>
-      <c r="N136">
-        <v>3292.64</v>
-      </c>
-      <c r="O136">
-        <v>7.5</v>
-      </c>
-      <c r="Q136">
-        <f t="shared" si="4"/>
-        <v>53.5</v>
-      </c>
-      <c r="R136">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S136">
-        <f t="shared" si="6"/>
-        <v>7.5</v>
-      </c>
-      <c r="T136" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869745370372</v>
-      </c>
-    </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>42695.86986111111</v>
-      </c>
-      <c r="B137">
-        <v>53</v>
-      </c>
-      <c r="C137">
-        <v>51</v>
-      </c>
-      <c r="F137">
-        <v>52</v>
-      </c>
-      <c r="G137">
-        <v>105</v>
-      </c>
-      <c r="H137">
-        <v>1</v>
-      </c>
-      <c r="I137">
-        <v>3292.64</v>
-      </c>
-      <c r="K137">
-        <v>49</v>
-      </c>
-      <c r="L137">
-        <v>103</v>
-      </c>
-      <c r="M137">
-        <v>0</v>
-      </c>
-      <c r="N137">
-        <v>3292.64</v>
-      </c>
-      <c r="O137">
-        <v>7.4</v>
-      </c>
-      <c r="Q137">
-        <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="R137">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="S137">
-        <f t="shared" si="6"/>
-        <v>7.4</v>
-      </c>
-      <c r="T137" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.86986111111</v>
-      </c>
-    </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <v>42695.869976851849</v>
-      </c>
-      <c r="B138">
-        <v>53</v>
-      </c>
-      <c r="C138">
-        <v>51</v>
-      </c>
-      <c r="F138">
-        <v>52</v>
-      </c>
-      <c r="G138">
-        <v>105</v>
-      </c>
-      <c r="H138">
-        <v>0</v>
-      </c>
-      <c r="I138">
-        <v>3292.64</v>
-      </c>
-      <c r="K138">
-        <v>49</v>
-      </c>
-      <c r="L138">
-        <v>103</v>
-      </c>
-      <c r="M138">
-        <v>0</v>
-      </c>
-      <c r="N138">
-        <v>3292.64</v>
-      </c>
-      <c r="O138">
-        <v>7.4</v>
-      </c>
-      <c r="Q138">
-        <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="R138">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S138">
-        <f t="shared" si="6"/>
-        <v>7.4</v>
-      </c>
-      <c r="T138" s="2">
-        <f t="shared" si="7"/>
-        <v>42695.869976851849</v>
-      </c>
-    </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>42695.870092592595</v>
-      </c>
-      <c r="B139">
-        <v>54</v>
-      </c>
-      <c r="C139">
-        <v>51</v>
-      </c>
-      <c r="F139">
-        <v>52</v>
-      </c>
-      <c r="G139">
-        <v>105</v>
-      </c>
-      <c r="H139">
-        <v>0</v>
-      </c>
-      <c r="I139">
-        <v>3292.64</v>
-      </c>
-      <c r="K139">
-        <v>49</v>
-      </c>
-      <c r="L139">
-        <v>103</v>
-      </c>
-      <c r="M139">
-        <v>0</v>
-      </c>
-      <c r="N139">
-        <v>3292.64</v>
-      </c>
-      <c r="O139">
-        <v>7.4</v>
-      </c>
-      <c r="Q139">
-        <f t="shared" ref="Q139:Q150" si="8">AVERAGE(B139:C139)</f>
-        <v>52.5</v>
-      </c>
-      <c r="R139">
-        <f t="shared" ref="R139:R150" si="9" xml:space="preserve"> AVERAGE(H139,M139)</f>
-        <v>0</v>
-      </c>
-      <c r="S139">
-        <f t="shared" ref="S139:S150" si="10">O139</f>
-        <v>7.4</v>
-      </c>
-      <c r="T139" s="2">
-        <f t="shared" ref="T139:T150" si="11">A139</f>
-        <v>42695.870092592595</v>
-      </c>
-    </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <v>42695.870208333334</v>
-      </c>
-      <c r="B140">
-        <v>53</v>
-      </c>
-      <c r="C140">
-        <v>51</v>
-      </c>
-      <c r="F140">
-        <v>51</v>
-      </c>
-      <c r="G140">
-        <v>105</v>
-      </c>
-      <c r="H140">
-        <v>0</v>
-      </c>
-      <c r="I140">
-        <v>3292.64</v>
-      </c>
-      <c r="K140">
-        <v>49</v>
-      </c>
-      <c r="L140">
-        <v>103</v>
-      </c>
-      <c r="M140">
-        <v>0</v>
-      </c>
-      <c r="N140">
-        <v>3292.64</v>
-      </c>
-      <c r="O140">
-        <v>7.5</v>
-      </c>
-      <c r="Q140">
-        <f t="shared" si="8"/>
-        <v>52</v>
-      </c>
-      <c r="R140">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S140">
-        <f t="shared" si="10"/>
-        <v>7.5</v>
-      </c>
-      <c r="T140" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870208333334</v>
-      </c>
-    </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>42695.870324074072</v>
-      </c>
-      <c r="B141">
-        <v>53</v>
-      </c>
-      <c r="C141">
-        <v>52</v>
-      </c>
-      <c r="F141">
-        <v>51</v>
-      </c>
-      <c r="G141">
-        <v>105</v>
-      </c>
-      <c r="H141">
-        <v>0</v>
-      </c>
-      <c r="I141">
-        <v>3292.64</v>
-      </c>
-      <c r="K141">
-        <v>49</v>
-      </c>
-      <c r="L141">
-        <v>103</v>
-      </c>
-      <c r="M141">
-        <v>0</v>
-      </c>
-      <c r="N141">
-        <v>3292.64</v>
-      </c>
-      <c r="O141">
-        <v>7.5</v>
-      </c>
-      <c r="Q141">
-        <f t="shared" si="8"/>
-        <v>52.5</v>
-      </c>
-      <c r="R141">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S141">
-        <f t="shared" si="10"/>
-        <v>7.5</v>
-      </c>
-      <c r="T141" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870324074072</v>
-      </c>
-    </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>42695.870439814818</v>
-      </c>
-      <c r="B142">
-        <v>52</v>
-      </c>
-      <c r="C142">
-        <v>50</v>
-      </c>
-      <c r="F142">
-        <v>51</v>
-      </c>
-      <c r="G142">
-        <v>105</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
-      </c>
-      <c r="I142">
-        <v>3292.64</v>
-      </c>
-      <c r="K142">
-        <v>49</v>
-      </c>
-      <c r="L142">
-        <v>103</v>
-      </c>
-      <c r="M142">
-        <v>0</v>
-      </c>
-      <c r="N142">
-        <v>3292.64</v>
-      </c>
-      <c r="O142">
-        <v>7.4</v>
-      </c>
-      <c r="Q142">
-        <f t="shared" si="8"/>
-        <v>51</v>
-      </c>
-      <c r="R142">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S142">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T142" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870439814818</v>
-      </c>
-    </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <v>42695.870555555557</v>
-      </c>
-      <c r="B143">
-        <v>52</v>
-      </c>
-      <c r="C143">
-        <v>50</v>
-      </c>
-      <c r="F143">
-        <v>49</v>
-      </c>
-      <c r="G143">
-        <v>105</v>
-      </c>
-      <c r="H143">
-        <v>0</v>
-      </c>
-      <c r="I143">
-        <v>3292.64</v>
-      </c>
-      <c r="K143">
-        <v>49</v>
-      </c>
-      <c r="L143">
-        <v>103</v>
-      </c>
-      <c r="M143">
-        <v>1</v>
-      </c>
-      <c r="N143">
-        <v>3292.64</v>
-      </c>
-      <c r="O143">
-        <v>7.5</v>
-      </c>
-      <c r="Q143">
-        <f t="shared" si="8"/>
-        <v>51</v>
-      </c>
-      <c r="R143">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
-      <c r="S143">
-        <f t="shared" si="10"/>
-        <v>7.5</v>
-      </c>
-      <c r="T143" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870555555557</v>
-      </c>
-    </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>42695.870671296296</v>
-      </c>
-      <c r="B144">
-        <v>51</v>
-      </c>
-      <c r="C144">
-        <v>48</v>
-      </c>
-      <c r="F144">
-        <v>49</v>
-      </c>
-      <c r="G144">
-        <v>105</v>
-      </c>
-      <c r="H144">
-        <v>0</v>
-      </c>
-      <c r="I144">
-        <v>3292.64</v>
-      </c>
-      <c r="K144">
-        <v>48</v>
-      </c>
-      <c r="L144">
-        <v>103</v>
-      </c>
-      <c r="M144">
-        <v>0</v>
-      </c>
-      <c r="N144">
-        <v>3292.64</v>
-      </c>
-      <c r="O144">
-        <v>7.4</v>
-      </c>
-      <c r="Q144">
-        <f t="shared" si="8"/>
-        <v>49.5</v>
-      </c>
-      <c r="R144">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S144">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T144" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870671296296</v>
-      </c>
-    </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>42695.870787037034</v>
-      </c>
-      <c r="B145">
-        <v>50</v>
-      </c>
-      <c r="C145">
-        <v>49</v>
-      </c>
-      <c r="F145">
-        <v>49</v>
-      </c>
-      <c r="G145">
-        <v>105</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-      <c r="I145">
-        <v>3292.64</v>
-      </c>
-      <c r="K145">
-        <v>48</v>
-      </c>
-      <c r="L145">
-        <v>103</v>
-      </c>
-      <c r="M145">
-        <v>0</v>
-      </c>
-      <c r="N145">
-        <v>3292.64</v>
-      </c>
-      <c r="O145">
-        <v>7.4</v>
-      </c>
-      <c r="Q145">
-        <f t="shared" si="8"/>
-        <v>49.5</v>
-      </c>
-      <c r="R145">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S145">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T145" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.870787037034</v>
-      </c>
-    </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>42695.87090277778</v>
-      </c>
-      <c r="B146">
-        <v>49</v>
-      </c>
-      <c r="C146">
-        <v>48</v>
-      </c>
-      <c r="F146">
-        <v>49</v>
-      </c>
-      <c r="G146">
-        <v>105</v>
-      </c>
-      <c r="H146">
-        <v>0</v>
-      </c>
-      <c r="I146">
-        <v>3292.64</v>
-      </c>
-      <c r="K146">
-        <v>48</v>
-      </c>
-      <c r="L146">
-        <v>103</v>
-      </c>
-      <c r="M146">
-        <v>0</v>
-      </c>
-      <c r="N146">
-        <v>3292.64</v>
-      </c>
-      <c r="O146">
-        <v>7.4</v>
-      </c>
-      <c r="Q146">
-        <f t="shared" si="8"/>
-        <v>48.5</v>
-      </c>
-      <c r="R146">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S146">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T146" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.87090277778</v>
-      </c>
-    </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>42695.871018518519</v>
-      </c>
-      <c r="B147">
-        <v>50</v>
-      </c>
-      <c r="C147">
-        <v>49</v>
-      </c>
-      <c r="F147">
-        <v>48</v>
-      </c>
-      <c r="G147">
-        <v>105</v>
-      </c>
-      <c r="H147">
-        <v>0</v>
-      </c>
-      <c r="I147">
-        <v>3292.64</v>
-      </c>
-      <c r="K147">
-        <v>48</v>
-      </c>
-      <c r="L147">
-        <v>103</v>
-      </c>
-      <c r="M147">
-        <v>0</v>
-      </c>
-      <c r="N147">
-        <v>3292.64</v>
-      </c>
-      <c r="O147">
-        <v>7.4</v>
-      </c>
-      <c r="Q147">
-        <f t="shared" si="8"/>
-        <v>49.5</v>
-      </c>
-      <c r="R147">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S147">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T147" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.871018518519</v>
-      </c>
-    </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>42695.871134259258</v>
-      </c>
-      <c r="B148">
-        <v>48</v>
-      </c>
-      <c r="C148">
-        <v>48</v>
-      </c>
-      <c r="F148">
-        <v>48</v>
-      </c>
-      <c r="G148">
-        <v>105</v>
-      </c>
-      <c r="H148">
-        <v>0</v>
-      </c>
-      <c r="I148">
-        <v>3292.64</v>
-      </c>
-      <c r="K148">
-        <v>48</v>
-      </c>
-      <c r="L148">
-        <v>103</v>
-      </c>
-      <c r="M148">
-        <v>0</v>
-      </c>
-      <c r="N148">
-        <v>3292.64</v>
-      </c>
-      <c r="O148">
-        <v>7.4</v>
-      </c>
-      <c r="Q148">
-        <f t="shared" si="8"/>
-        <v>48</v>
-      </c>
-      <c r="R148">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S148">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T148" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.871134259258</v>
-      </c>
-    </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>42695.871249999997</v>
-      </c>
-      <c r="B149">
-        <v>50</v>
-      </c>
-      <c r="C149">
-        <v>49</v>
-      </c>
-      <c r="F149">
-        <v>48</v>
-      </c>
-      <c r="G149">
-        <v>105</v>
-      </c>
-      <c r="H149">
-        <v>1</v>
-      </c>
-      <c r="I149">
-        <v>3292.64</v>
-      </c>
-      <c r="K149">
-        <v>48</v>
-      </c>
-      <c r="L149">
-        <v>103</v>
-      </c>
-      <c r="M149">
-        <v>0</v>
-      </c>
-      <c r="N149">
-        <v>3292.64</v>
-      </c>
-      <c r="O149">
-        <v>7.4</v>
-      </c>
-      <c r="Q149">
-        <f t="shared" si="8"/>
-        <v>49.5</v>
-      </c>
-      <c r="R149">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
-      <c r="S149">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T149" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.871249999997</v>
-      </c>
-    </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>42695.871365740742</v>
-      </c>
-      <c r="B150">
-        <v>48</v>
-      </c>
-      <c r="C150">
-        <v>48</v>
-      </c>
-      <c r="F150">
-        <v>48</v>
-      </c>
-      <c r="G150">
-        <v>105</v>
-      </c>
-      <c r="H150">
-        <v>0</v>
-      </c>
-      <c r="I150">
-        <v>3292.64</v>
-      </c>
-      <c r="K150">
-        <v>46</v>
-      </c>
-      <c r="L150">
-        <v>103</v>
-      </c>
-      <c r="M150">
-        <v>0</v>
-      </c>
-      <c r="N150">
-        <v>3292.64</v>
-      </c>
-      <c r="O150">
-        <v>7.4</v>
-      </c>
-      <c r="Q150">
-        <f t="shared" si="8"/>
-        <v>48</v>
-      </c>
-      <c r="R150">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="S150">
-        <f t="shared" si="10"/>
-        <v>7.4</v>
-      </c>
-      <c r="T150" s="2">
-        <f t="shared" si="11"/>
-        <v>42695.871365740742</v>
-      </c>
-    </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+      <c r="T111" s="2"/>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="T112" s="2"/>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+      <c r="T113" s="2"/>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="T114" s="2"/>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+      <c r="T115" s="2"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="T116" s="2"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+      <c r="T117" s="2"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="T118" s="2"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="T119" s="2"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="T120" s="2"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+      <c r="T121" s="2"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+      <c r="T122" s="2"/>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+      <c r="T123" s="2"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="T124" s="2"/>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="T125" s="2"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="T126" s="2"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="T127" s="2"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+      <c r="T128" s="2"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="T129" s="2"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="T130" s="2"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="T131" s="2"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+      <c r="T132" s="2"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="T133" s="2"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+      <c r="T134" s="2"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="T135" s="2"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+      <c r="T136" s="2"/>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="T137" s="2"/>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+      <c r="T138" s="2"/>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="T139" s="2"/>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A140" s="1"/>
+      <c r="T140" s="2"/>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+      <c r="T141" s="2"/>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A142" s="1"/>
+      <c r="T142" s="2"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A143" s="1"/>
+      <c r="T143" s="2"/>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="T144" s="2"/>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A145" s="1"/>
+      <c r="T145" s="2"/>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A146" s="1"/>
+      <c r="T146" s="2"/>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A147" s="1"/>
+      <c r="T147" s="2"/>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A148" s="1"/>
+      <c r="T148" s="2"/>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A149" s="1"/>
+      <c r="T149" s="2"/>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A150" s="1"/>
+      <c r="T150" s="2"/>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="1"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="1"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="1"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="1"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="1"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="1"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="1"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="1"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="1"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="1"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="1"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="1"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="1"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="1"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="1"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="1"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" s="1"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="1"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="1"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="1"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="1"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="1"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="1"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="1"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="1"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="1"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="1"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="1"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="1"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="1"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="1"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="1"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="1"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="1"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="1"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="1"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="1"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="1"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="1"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="1"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="1"/>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="1"/>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>22</v>
       </c>

</xml_diff>